<commit_message>
Added LRelu raw networks
</commit_message>
<xml_diff>
--- a/docs/Raw agents summary.xlsx
+++ b/docs/Raw agents summary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Hidden layer = 40 neurons</t>
   </si>
@@ -112,6 +112,27 @@
   </si>
   <si>
     <t>Raw-GnuBg-40-relu</t>
+  </si>
+  <si>
+    <t>Raw-Sutton-40-lrelu</t>
+  </si>
+  <si>
+    <t>Lrelu</t>
+  </si>
+  <si>
+    <t>Raw-Tesauro89-40-lrelu</t>
+  </si>
+  <si>
+    <t>Raw-Tesauro92-40-lrelu</t>
+  </si>
+  <si>
+    <t>Raw-GnuBg-40-lrelu</t>
+  </si>
+  <si>
+    <t>Raw-Sutton-40-elu</t>
+  </si>
+  <si>
+    <t>Elu</t>
   </si>
 </sst>
 </file>
@@ -167,8 +188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:I15" totalsRowShown="0">
-  <autoFilter ref="A3:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:I23" totalsRowShown="0">
+  <autoFilter ref="A3:I23"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Agent Name"/>
     <tableColumn id="2" name="Activation"/>
@@ -481,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,6 +901,157 @@
       </c>
       <c r="I15">
         <v>1.4070138948036499E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>319</v>
+      </c>
+      <c r="E16">
+        <v>1.0033394684030699E-2</v>
+      </c>
+      <c r="F16">
+        <v>352</v>
+      </c>
+      <c r="G16">
+        <v>3.11701877751514E-2</v>
+      </c>
+      <c r="H16">
+        <v>308</v>
+      </c>
+      <c r="I16">
+        <v>1.78892986171405E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>165</v>
+      </c>
+      <c r="E17">
+        <v>8.5945415559447805E-3</v>
+      </c>
+      <c r="F17">
+        <v>187</v>
+      </c>
+      <c r="G17">
+        <v>1.44900887994673E-2</v>
+      </c>
+      <c r="H17">
+        <v>165</v>
+      </c>
+      <c r="I17">
+        <v>1.1670147232056199E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>165</v>
+      </c>
+      <c r="E18">
+        <v>9.1649879250330201E-3</v>
+      </c>
+      <c r="F18">
+        <v>254</v>
+      </c>
+      <c r="G18">
+        <v>1.4580407029913801E-2</v>
+      </c>
+      <c r="H18">
+        <v>198</v>
+      </c>
+      <c r="I18">
+        <v>1.38817468289366E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>220</v>
+      </c>
+      <c r="E19">
+        <v>9.19357906345529E-3</v>
+      </c>
+      <c r="F19">
+        <v>253</v>
+      </c>
+      <c r="G19">
+        <v>1.4600829719728E-2</v>
+      </c>
+      <c r="H19">
+        <v>143</v>
+      </c>
+      <c r="I19">
+        <v>1.7127940607985E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>